<commit_message>
task 2 and 1a
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofik\Documents\Uni Konstanz\SEDS\SoSe 24\Data Visualizations\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035BDB08-7316-491B-9FB9-5B207CDFDA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83C8A9D-5AAA-456C-A127-038751FDDBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Exercise</t>
   </si>
@@ -55,14 +55,45 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">task 1: 9.5/10
+- d) What about shape? explicitly mention position, color and shape in relationship to similarity and proximity
+task 2: 9.5/10
+- initialisation of scatterplot does not work properly
+</t>
+  </si>
+  <si>
+    <t>Over</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>90% for 0.3 bonus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,17 +118,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,52 +410,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="85.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="85.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -428,51 +467,79 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B13">
         <f>SUM(B2:B11)</f>
-        <v>56</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f>COUNT(B2:B11)*20</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
+        <f>B13/B14</f>
+        <v>0.9375</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
task 1 - theory
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofik\Documents\Uni Konstanz\SEDS\SoSe 24\Data Visualizations\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83C8A9D-5AAA-456C-A127-038751FDDBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3270D079-5EBB-46D9-9155-C4EDA5DE47CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -413,17 +413,17 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="85.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="3" width="9.26953125" customWidth="1"/>
+    <col min="4" max="4" width="85.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -437,7 +437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -448,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -467,7 +467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -478,61 +478,67 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B13">
         <f>SUM(B2:B11)</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B14">
         <f>COUNT(B2:B11)*20</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2">
         <f>B13/B14</f>
-        <v>0.9375</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>

</xml_diff>